<commit_message>
updated cloth whale resource pack
</commit_message>
<xml_diff>
--- a/RESOURCEPACKS/CLOTH_WHALE_BLOCKS/Book1.xlsx
+++ b/RESOURCEPACKS/CLOTH_WHALE_BLOCKS/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.minecraft\resourcepacks\CLOTH_WHALE_BANNERS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F71C67-4FDA-4A55-B2DB-6FCC2447333E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4671EB87-C501-4DFF-B493-40DB9BB6C915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8700" yWindow="210" windowWidth="19995" windowHeight="11340" xr2:uid="{22E7FEB1-27A7-4E3B-BE20-B3A988BAD67A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>u1</t>
   </si>
@@ -57,7 +57,10 @@
     <t>new</t>
   </si>
   <si>
-    <t>old</t>
+    <t>Top-Left Symbol</t>
+  </si>
+  <si>
+    <t>copy&amp;paste</t>
   </si>
 </sst>
 </file>
@@ -409,19 +412,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61C730A-DA8F-4BF5-9304-500B0C2F3157}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="K5" sqref="K5:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -429,7 +433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -460,8 +464,11 @@
       <c r="J2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.069</v>
       </c>
@@ -481,23 +488,27 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G4:G24" si="0">A5+(E5*1.173)</f>
+        <f t="shared" ref="G5:G24" si="0">A5+(E5*1.173)</f>
         <v>1.069</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H4:H24" si="1">B5+(F5*1.28)</f>
+        <f t="shared" ref="H5:H24" si="1">B5+(F5*1.28)</f>
         <v>1.8130000000000002</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I4:I24" si="2">C5+(E5*1.173)</f>
+        <f t="shared" ref="I5:I24" si="2">C5+(E5*1.173)</f>
         <v>2.0259999999999998</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J4:J24" si="3">D5+(F5*1.28)</f>
+        <f t="shared" ref="J5:J24" si="3">D5+(F5*1.28)</f>
         <v>2.774</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="str">
+        <f>CONCATENATE(G5,", ",H5,", ",I5,", ",J5)</f>
+        <v>1.069, 1.813, 2.026, 2.774</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.069</v>
       </c>
@@ -529,8 +540,12 @@
         <f t="shared" si="3"/>
         <v>4.0540000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="str">
+        <f t="shared" ref="K6:K41" si="4">CONCATENATE(G6,", ",H6,", ",I6,", ",J6)</f>
+        <v>1.069, 3.093, 2.026, 4.054</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1.069</v>
       </c>
@@ -562,8 +577,12 @@
         <f t="shared" si="3"/>
         <v>5.3339999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>1.069, 4.373, 2.026, 5.334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.069</v>
       </c>
@@ -595,8 +614,12 @@
         <f t="shared" si="3"/>
         <v>6.6139999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>1.069, 5.653, 2.026, 6.614</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.069</v>
       </c>
@@ -628,8 +651,12 @@
         <f t="shared" si="3"/>
         <v>7.8940000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>1.069, 6.933, 2.026, 7.894</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.069</v>
       </c>
@@ -661,8 +688,12 @@
         <f t="shared" si="3"/>
         <v>9.1739999999999995</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
+        <v>1.069, 8.213, 2.026, 9.174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.069</v>
       </c>
@@ -694,8 +725,12 @@
         <f t="shared" si="3"/>
         <v>10.454000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>1.069, 9.493, 2.026, 10.454</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.069</v>
       </c>
@@ -727,8 +762,12 @@
         <f t="shared" si="3"/>
         <v>11.734</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>1.069, 10.773, 2.026, 11.734</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.069</v>
       </c>
@@ -760,8 +799,12 @@
         <f t="shared" si="3"/>
         <v>13.013999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
+        <v>1.069, 12.053, 2.026, 13.014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.069</v>
       </c>
@@ -793,8 +836,12 @@
         <f t="shared" si="3"/>
         <v>14.294</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
+        <v>1.069, 13.333, 2.026, 14.294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.069</v>
       </c>
@@ -826,8 +873,12 @@
         <f t="shared" si="3"/>
         <v>15.574</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
+        <v>1.069, 14.613, 2.026, 15.574</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.069</v>
       </c>
@@ -862,8 +913,12 @@
         <f t="shared" si="3"/>
         <v>11.734</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
+        <v>9.28, 10.773, 10.237, 11.734</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.069</v>
       </c>
@@ -898,8 +953,12 @@
         <f t="shared" si="3"/>
         <v>4.0540000000000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 3.093, 3.199, 4.054</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.069</v>
       </c>
@@ -934,8 +993,12 @@
         <f t="shared" si="3"/>
         <v>5.3339999999999996</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 4.373, 3.199, 5.334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.069</v>
       </c>
@@ -970,8 +1033,12 @@
         <f t="shared" si="3"/>
         <v>6.6139999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 5.653, 3.199, 6.614</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.069</v>
       </c>
@@ -1006,8 +1073,12 @@
         <f t="shared" si="3"/>
         <v>7.8940000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 6.933, 3.199, 7.894</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.069</v>
       </c>
@@ -1042,8 +1113,12 @@
         <f t="shared" si="3"/>
         <v>9.1739999999999995</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 8.213, 3.199, 9.174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1.069</v>
       </c>
@@ -1078,8 +1153,12 @@
         <f t="shared" si="3"/>
         <v>10.454000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 9.493, 3.199, 10.454</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1.069</v>
       </c>
@@ -1114,8 +1193,12 @@
         <f t="shared" si="3"/>
         <v>11.734</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 10.773, 3.199, 11.734</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1.069</v>
       </c>
@@ -1150,8 +1233,12 @@
         <f t="shared" si="3"/>
         <v>13.013999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 12.053, 3.199, 13.014</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1.069</v>
       </c>
@@ -1171,23 +1258,27 @@
         <v>10</v>
       </c>
       <c r="G25">
-        <f t="shared" ref="G25:G27" si="4">A25+(E25*1.173)</f>
+        <f t="shared" ref="G25:G28" si="5">A25+(E25*1.173)</f>
         <v>2.242</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25:H27" si="5">B25+(F25*1.28)</f>
+        <f t="shared" ref="H25:H28" si="6">B25+(F25*1.28)</f>
         <v>13.333</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:I27" si="6">C25+(E25*1.173)</f>
+        <f t="shared" ref="I25:I28" si="7">C25+(E25*1.173)</f>
         <v>3.1989999999999998</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:J27" si="7">D25+(F25*1.28)</f>
+        <f t="shared" ref="J25:J28" si="8">D25+(F25*1.28)</f>
         <v>14.294</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 13.333, 3.199, 14.294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1.069</v>
       </c>
@@ -1207,23 +1298,27 @@
         <v>11</v>
       </c>
       <c r="G26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.242</v>
       </c>
       <c r="H26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14.613</v>
       </c>
       <c r="I26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.1989999999999998</v>
       </c>
       <c r="J26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15.574</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 14.613, 3.199, 15.574</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1.069</v>
       </c>
@@ -1243,20 +1338,584 @@
         <v>12</v>
       </c>
       <c r="G27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.242</v>
       </c>
       <c r="H27">
+        <f t="shared" si="6"/>
+        <v>15.892999999999999</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="7"/>
+        <v>3.1989999999999998</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="8"/>
+        <v>16.853999999999999</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="4"/>
+        <v>2.242, 15.893, 3.199, 16.854</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1.069</v>
+      </c>
+      <c r="B28">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C28">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D28">
+        <v>1.494</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="5"/>
+        <v>3.415</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="6"/>
+        <v>1.8130000000000002</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="7"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="8"/>
+        <v>2.774</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 1.813, 4.372, 2.774</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1.069</v>
+      </c>
+      <c r="B29">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C29">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D29">
+        <v>1.494</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:G41" si="9">A29+(E29*1.173)</f>
+        <v>3.415</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ref="H29:H41" si="10">B29+(F29*1.28)</f>
+        <v>3.093</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ref="I29:I41" si="11">C29+(E29*1.173)</f>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J29">
+        <f t="shared" ref="J29:J41" si="12">D29+(F29*1.28)</f>
+        <v>4.0540000000000003</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 3.093, 4.372, 4.054</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1.069</v>
+      </c>
+      <c r="B30">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C30">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D30">
+        <v>1.494</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="10"/>
+        <v>4.3730000000000002</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="12"/>
+        <v>5.3339999999999996</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 4.373, 4.372, 5.334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1.069</v>
+      </c>
+      <c r="B31">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C31">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D31">
+        <v>1.494</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="10"/>
+        <v>5.6530000000000005</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="12"/>
+        <v>6.6139999999999999</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 5.653, 4.372, 6.614</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1.069</v>
+      </c>
+      <c r="B32">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C32">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D32">
+        <v>1.494</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="10"/>
+        <v>6.9330000000000007</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="12"/>
+        <v>7.8940000000000001</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 6.933, 4.372, 7.894</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1.069</v>
+      </c>
+      <c r="B33">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C33">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D33">
+        <v>1.494</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="10"/>
+        <v>8.2129999999999992</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="12"/>
+        <v>9.1739999999999995</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 8.213, 4.372, 9.174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1.069</v>
+      </c>
+      <c r="B34">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C34">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D34">
+        <v>1.494</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>7</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="10"/>
+        <v>9.4930000000000003</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="12"/>
+        <v>10.454000000000001</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 9.493, 4.372, 10.454</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1.069</v>
+      </c>
+      <c r="B35">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C35">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D35">
+        <v>1.494</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="10"/>
+        <v>10.773</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="12"/>
+        <v>11.734</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 10.773, 4.372, 11.734</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1.069</v>
+      </c>
+      <c r="B36">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C36">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D36">
+        <v>1.494</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>9</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="10"/>
+        <v>12.052999999999999</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="12"/>
+        <v>13.013999999999999</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 12.053, 4.372, 13.014</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1.069</v>
+      </c>
+      <c r="B37">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C37">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D37">
+        <v>1.494</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="10"/>
+        <v>13.333</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="12"/>
+        <v>14.294</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 13.333, 4.372, 14.294</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1.069</v>
+      </c>
+      <c r="B38">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C38">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D38">
+        <v>1.494</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>11</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="10"/>
+        <v>14.613</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="12"/>
+        <v>15.574</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 14.613, 4.372, 15.574</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1.069</v>
+      </c>
+      <c r="B39">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C39">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D39">
+        <v>1.494</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>12</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="10"/>
         <v>15.892999999999999</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="6"/>
-        <v>3.1989999999999998</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="7"/>
+      <c r="I39">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="12"/>
         <v>16.853999999999999</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 15.893, 4.372, 16.854</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1.069</v>
+      </c>
+      <c r="B40">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C40">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D40">
+        <v>1.494</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>13</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="10"/>
+        <v>17.173000000000002</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="12"/>
+        <v>18.134</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 17.173, 4.372, 18.134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1.069</v>
+      </c>
+      <c r="B41">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C41">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="D41">
+        <v>1.494</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>14</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="9"/>
+        <v>3.415</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="10"/>
+        <v>18.453000000000003</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="11"/>
+        <v>4.3719999999999999</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="12"/>
+        <v>19.414000000000001</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="4"/>
+        <v>3.415, 18.453, 4.372, 19.414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>